<commit_message>
se modifica la forma de cargar datos para realizar las consultas del back y mejorar los features en redaccion
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Autenticacion.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Autenticacion.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7695"/>
+    <workbookView windowWidth="20490" windowHeight="7695" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
-    <sheet name="Listas" sheetId="2" r:id="rId2"/>
+    <sheet name="Transaccion" sheetId="3" r:id="rId2"/>
+    <sheet name="Listas" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -184,10 +185,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -214,6 +215,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -221,16 +253,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -243,85 +268,45 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -342,6 +327,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -351,14 +359,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -397,19 +398,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,157 +572,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -609,6 +610,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -620,50 +630,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -684,6 +650,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -697,152 +687,163 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1182,7 +1183,7 @@
   <sheetPr/>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -1482,6 +1483,99 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:D7"/>

</xml_diff>

<commit_message>
Quitar comentarios en las clases
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Autenticacion.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Autenticacion.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -107,9 +107,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>001</t>
-  </si>
-  <si>
     <t>CONSULTAR_PRODUCTO</t>
   </si>
   <si>
@@ -186,6 +183,21 @@
   </si>
   <si>
     <t>43024987</t>
+  </si>
+  <si>
+    <t>Alterno</t>
+  </si>
+  <si>
+    <t>052</t>
+  </si>
+  <si>
+    <t>CLAVE NO VALIDA</t>
+  </si>
+  <si>
+    <t>Clave bloqueada</t>
+  </si>
+  <si>
+    <t>607</t>
   </si>
 </sst>
 </file>
@@ -288,21 +300,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,12 +591,19 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="13" max="13" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="6" width="11" style="8"/>
+    <col min="7" max="8" width="13.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="8"/>
+    <col min="10" max="10" width="20.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -627,45 +643,45 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="M2" s="3" t="s">
@@ -673,40 +689,40 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="3" t="s">
@@ -714,7 +730,7 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -723,7 +739,7 @@
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -736,9 +752,9 @@
         <v>18</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>20</v>
       </c>
       <c r="J4" s="3" t="s">
@@ -751,130 +767,130 @@
         <v>23</v>
       </c>
       <c r="M4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="8" t="s">
+      <c r="B5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="9" t="s">
+      <c r="G7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="M5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="8" t="s">
+      <c r="M7" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M7" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -930,46 +946,46 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="12" customFormat="1">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:12" s="8" customFormat="1">
+      <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="E3" s="13"/>
+      <c r="E3" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -994,16 +1010,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>39</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1011,50 +1027,50 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
         <v>44</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>46</v>
-      </c>
-      <c r="D3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
         <v>48</v>
-      </c>
-      <c r="D4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se arregla seleccion de menu y modifica data para estabilizacion
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Autenticacion.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Autenticacion.xlsx
@@ -1,32 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/Proyectos TODO1/bancolombia-app-personas-osp-tests-bdd-screen-play/APP_PERSONAS/src/test/resources/datadriven/autenticacion/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20500" windowHeight="7700"/>
+    <workbookView windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
-    <sheet name="Transaccion" sheetId="3" r:id="rId2"/>
-    <sheet name="Listas" sheetId="2" r:id="rId3"/>
+    <sheet name="Listas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -133,10 +122,10 @@
     <t>6</t>
   </si>
   <si>
-    <t>95400152</t>
-  </si>
-  <si>
-    <t>sandrita69</t>
+    <t>10757877</t>
+  </si>
+  <si>
+    <t>usrblocked01</t>
   </si>
   <si>
     <t>0370</t>
@@ -193,20 +182,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -224,8 +212,159 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,8 +389,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -274,29 +599,320 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="Normal 2" xfId="32"/>
+    <cellStyle name="20% - Accent5" xfId="33" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="34" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="35" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="36" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="38" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="39" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="40" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="41" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="42" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="43" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="44" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="45" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="46" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="47" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="48" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="49" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -558,24 +1174,24 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="6"/>
   <cols>
-    <col min="13" max="13" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -612,250 +1228,250 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:13">
+      <c r="A2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:13">
+      <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:13">
+      <c r="A4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:13">
+      <c r="A5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="11" t="s">
         <v>23</v>
       </c>
       <c r="M5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:13">
+      <c r="A6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="11" t="s">
         <v>23</v>
       </c>
       <c r="M6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:13">
+      <c r="A7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="10" t="s">
         <v>23</v>
       </c>
       <c r="M7" t="s">
@@ -864,117 +1480,28 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="14.8333333333333" customWidth="1"/>
+    <col min="3" max="3" width="12.1666666666667" customWidth="1"/>
+    <col min="4" max="4" width="17.8333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -988,7 +1515,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1002,7 +1529,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1016,7 +1543,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4">
       <c r="B4" t="s">
         <v>49</v>
       </c>
@@ -1024,22 +1551,23 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:2">
       <c r="B6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:2">
       <c r="B7" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
estabilizacion de transacciones con data y task
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Autenticacion.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Autenticacion.xlsx
@@ -184,10 +184,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -213,38 +213,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -256,14 +243,104 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -272,32 +349,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -310,59 +363,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -391,187 +391,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -600,11 +600,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -633,17 +654,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -665,26 +682,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -700,15 +700,15 @@
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -718,131 +718,131 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1183,7 +1183,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="6"/>

</xml_diff>

<commit_message>
Se estabilizan features eliminando caracteres especiales y tildes
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Autenticacion.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Autenticacion.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AUTOMATIZACION JAVA\PROYECTOS GRADLE\PROYECTOS NUEVA APP\AW1059001_APPSucursalVirtualPersonas_Test\APP_PERSONAS\src\test\resources\datadriven\autenticacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosmarioloperamurillo/Documents/ProyectosIntellij/AW1059001_NuevaAPPSucursalVirtualPersonas_Test/APP_PERSONAS/src/test/resources/datadriven/autenticacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E847627E-E40D-5640-BBA8-39C79DB5F195}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27800" windowHeight="12700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -65,9 +66,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>1037655531</t>
-  </si>
-  <si>
     <t>userrobot1</t>
   </si>
   <si>
@@ -198,12 +196,15 @@
   </si>
   <si>
     <t>607</t>
+  </si>
+  <si>
+    <t>45612862</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="12"/>
@@ -224,14 +225,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -315,7 +316,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -587,22 +588,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="6" width="11" style="8"/>
     <col min="7" max="8" width="13.5" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="8"/>
-    <col min="10" max="10" width="20.375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
@@ -652,248 +653,248 @@
         <v>13</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="M3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="M4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="L5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="M5" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>14</v>
+        <v>29</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="K6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="M6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="J7" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="M7" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -902,14 +903,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
@@ -954,37 +955,37 @@
         <v>13</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -996,84 +997,84 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
-    <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>44</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>45</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
         <v>47</v>
-      </c>
-      <c r="D4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se cambia data para ruta critica y cambios en el feature
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Autenticacion.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Autenticacion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -63,97 +63,97 @@
     <t>43024987</t>
   </si>
   <si>
+    <t>autotest30</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>4321</t>
+  </si>
+  <si>
+    <t>Acierto</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>0369</t>
+  </si>
+  <si>
+    <t>NO ERROR</t>
+  </si>
+  <si>
+    <t>bolp</t>
+  </si>
+  <si>
+    <t>ACTIVO</t>
+  </si>
+  <si>
+    <t>EPREPAGO</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>45612862</t>
+  </si>
+  <si>
+    <t>TRANSFERIR_DINERO</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>CONSULTAR_PRODUCTO</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>testing10</t>
+  </si>
+  <si>
+    <t>1267</t>
+  </si>
+  <si>
+    <t>Alterno</t>
+  </si>
+  <si>
+    <t>052</t>
+  </si>
+  <si>
+    <t>CLAVE NO VALIDA</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>22493944</t>
+  </si>
+  <si>
+    <t>userrobot9</t>
+  </si>
+  <si>
+    <t>607</t>
+  </si>
+  <si>
+    <t>0370</t>
+  </si>
+  <si>
+    <t>Clave bloqueada</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>recaudosnatik66</t>
+  </si>
+  <si>
     <t>automata87</t>
-  </si>
-  <si>
-    <t>1234</t>
-  </si>
-  <si>
-    <t>4321</t>
-  </si>
-  <si>
-    <t>Acierto</t>
-  </si>
-  <si>
-    <t>000</t>
-  </si>
-  <si>
-    <t>0369</t>
-  </si>
-  <si>
-    <t>NO ERROR</t>
-  </si>
-  <si>
-    <t>bolp</t>
-  </si>
-  <si>
-    <t>ACTIVO</t>
-  </si>
-  <si>
-    <t>CONSULTAR_PRODUCTO</t>
-  </si>
-  <si>
-    <t>EPREPAGO</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>45612862</t>
-  </si>
-  <si>
-    <t>userrobot1</t>
-  </si>
-  <si>
-    <t>TRANSFERIR_DINERO</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>testing10</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>1267</t>
-  </si>
-  <si>
-    <t>Alterno</t>
-  </si>
-  <si>
-    <t>052</t>
-  </si>
-  <si>
-    <t>CLAVE NO VALIDA</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>22493944</t>
-  </si>
-  <si>
-    <t>userrobot9</t>
-  </si>
-  <si>
-    <t>607</t>
-  </si>
-  <si>
-    <t>0370</t>
-  </si>
-  <si>
-    <t>Clave bloqueada</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>recaudosnatik66</t>
   </si>
   <si>
     <t>Orientacion</t>
@@ -246,7 +246,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -281,6 +281,59 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -290,14 +343,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -315,30 +360,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -352,9 +374,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -367,27 +388,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -416,25 +416,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,157 +584,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -639,8 +639,38 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -648,8 +678,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -678,21 +708,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -704,21 +719,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -736,149 +736,149 @@
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1217,8 +1217,8 @@
   <sheetPr/>
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="7"/>
@@ -1314,22 +1314,20 @@
       <c r="M2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>16</v>
@@ -1356,21 +1354,21 @@
         <v>23</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>16</v>
@@ -1397,12 +1395,12 @@
         <v>23</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>14</v>
@@ -1411,7 +1409,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>16</v>
@@ -1438,15 +1436,15 @@
         <v>23</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>13</v>
@@ -1455,22 +1453,22 @@
         <v>32</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>20</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>22</v>
@@ -1479,21 +1477,21 @@
         <v>23</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>38</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>39</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>16</v>
@@ -1502,16 +1500,16 @@
         <v>17</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="J7" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>43</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>22</v>
@@ -1520,21 +1518,21 @@
         <v>23</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:12">
       <c r="A8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>16</v>
@@ -1543,10 +1541,10 @@
         <v>17</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>20</v>
@@ -1627,7 +1625,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
ejecucion ruta critica 14-01-2020
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Autenticacion.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Autenticacion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\OSP_NEW\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\autenticacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TODO1\OSP_NEW\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\autenticacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Prueba" sheetId="3" r:id="rId2"/>
     <sheet name="Listas" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -95,9 +95,6 @@
     <t>ACTIVO</t>
   </si>
   <si>
-    <t>EPREPAGO</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t>Consultas</t>
+  </si>
+  <si>
+    <t>INSCRIBIR_PRODUCTOS</t>
   </si>
 </sst>
 </file>
@@ -601,7 +601,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -697,16 +697,16 @@
         <v>23</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>13</v>
@@ -739,15 +739,15 @@
         <v>23</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>13</v>
@@ -780,12 +780,12 @@
         <v>23</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>14</v>
@@ -821,39 +821,39 @@
         <v>23</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>33</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>20</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>22</v>
@@ -862,21 +862,21 @@
         <v>23</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>38</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>16</v>
@@ -885,16 +885,16 @@
         <v>17</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="J7" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>22</v>
@@ -903,21 +903,21 @@
         <v>23</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>16</v>
@@ -926,10 +926,10 @@
         <v>17</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>20</v>
@@ -1008,7 +1008,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>16</v>
@@ -1061,16 +1061,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>48</v>
-      </c>
-      <c r="D1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1078,50 +1078,50 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>51</v>
-      </c>
-      <c r="D2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>54</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>55</v>
-      </c>
-      <c r="D3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
         <v>57</v>
-      </c>
-      <c r="D4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion data, objetos, steps, funcionalidad Autenticacion, plataformas Android, iOS
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Autenticacion.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/autenticacion/Autenticacion.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TODO1\OSP_NEW\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\autenticacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProyectosBCO\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\autenticacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9D3A6E-B7BC-4BB2-A72A-289CD6093D8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -116,9 +117,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>testing10</t>
-  </si>
-  <si>
     <t>1267</t>
   </si>
   <si>
@@ -128,27 +126,18 @@
     <t>052</t>
   </si>
   <si>
-    <t>CLAVE NO VALIDA</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
     <t>22493944</t>
   </si>
   <si>
-    <t>userrobot9</t>
-  </si>
-  <si>
     <t>607</t>
   </si>
   <si>
     <t>0370</t>
   </si>
   <si>
-    <t>Clave bloqueada</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
@@ -228,12 +217,24 @@
   </si>
   <si>
     <t>36625233</t>
+  </si>
+  <si>
+    <t>pruebauser01</t>
+  </si>
+  <si>
+    <t>bloqueotarjetas01</t>
+  </si>
+  <si>
+    <t>La clave que usas en el cajero está bloqueada</t>
+  </si>
+  <si>
+    <t>clave inválida</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="12"/>
@@ -360,7 +361,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -632,24 +633,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.3"/>
   <cols>
     <col min="1" max="1" width="11" style="1"/>
-    <col min="2" max="2" width="18.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="11" style="1"/>
-    <col min="7" max="8" width="13.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="1"/>
+    <col min="4" max="4" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11" style="1"/>
+    <col min="7" max="8" width="13.44140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1"/>
-    <col min="10" max="10" width="20.375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="38.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.6640625" style="1" customWidth="1"/>
     <col min="14" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
@@ -705,7 +708,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>16</v>
@@ -732,7 +735,7 @@
         <v>23</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N2" s="12"/>
     </row>
@@ -870,25 +873,25 @@
         <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>32</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>35</v>
+      <c r="J6" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>22</v>
@@ -902,16 +905,16 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>16</v>
@@ -920,16 +923,16 @@
         <v>17</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>22</v>
@@ -943,28 +946,28 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>20</v>
@@ -984,16 +987,16 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>16</v>
@@ -1002,10 +1005,10 @@
         <v>17</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>20</v>
@@ -1025,16 +1028,16 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>16</v>
@@ -1043,10 +1046,10 @@
         <v>17</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>20</v>
@@ -1066,16 +1069,16 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>16</v>
@@ -1084,10 +1087,10 @@
         <v>17</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>20</v>
@@ -1111,14 +1114,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.3"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
@@ -1169,7 +1172,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>16</v>
@@ -1205,33 +1208,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
-    <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1239,50 +1242,50 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>